<commit_message>
update notes before quarter ends, some receiables left
</commit_message>
<xml_diff>
--- a/2023_Q3/2023-Q3_羽球季打費用明細.xlsx
+++ b/2023_Q3/2023-Q3_羽球季打費用明細.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Docs\Private\週一豐東羽球團\2023_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCBC597-4DB8-425C-A0B2-74916BFC13C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD76525A-4A98-4391-A1CF-41045DB91E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="542" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
+    <workbookView xWindow="-88" yWindow="0" windowWidth="11484" windowHeight="12085" tabRatio="738" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
   </bookViews>
   <sheets>
     <sheet name="2023Q3羽球季費資訊" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>豐東場地費1900-2100時段 $420/小時</t>
   </si>
@@ -97,10 +97,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>=SUM(B2:C17)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>現金 2023Q2結餘</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -189,11 +185,38 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2023/07/10 更新餘額</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>7. 偉群 @吳偉群 (07/17 轉季繳 $120*10次 = $1200 未收)</t>
+    <t>現金 Frank友(鎮豪) 臨打費</t>
+  </si>
+  <si>
+    <t>現金 香菇、香菇友臨打費 (請鉉竣代收)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>應收</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 偉群 臨打費 (未收)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>=SUM(C21:C22)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/09/10 更新餘額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>=SUM(B2:C15)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>7.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>!! 08/07 當日整團請假，09/04 得知球場規定未能補打本季也即將結束，由 Ivy 額外提供兩桶新球為補償</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -207,7 +230,7 @@
     <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -294,6 +317,20 @@
     <font>
       <sz val="12"/>
       <color theme="4"/>
+      <name val="Microsoft JhengHei UI"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Microsoft JhengHei UI"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
       <name val="Microsoft JhengHei UI"/>
       <family val="2"/>
       <charset val="136"/>
@@ -345,7 +382,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -419,6 +456,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -741,159 +787,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35F76AE-921C-47CE-BB7E-B46F0098B109}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="40.125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.25" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.07421875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.23046875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18.55" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.55" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="32.700000000000003" x14ac:dyDescent="0.4">
+      <c r="A15" s="25" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1430</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="8">
-        <v>1430</v>
-      </c>
-      <c r="C16" s="9" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="6">
+        <v>120</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="6">
-        <v>120</v>
-      </c>
-      <c r="C18" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" s="2" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="5"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -905,21 +954,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCCEF2F-70B8-4CD5-8F32-AA2B6924B187}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.75" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="9.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.15234375" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>7</v>
       </c>
@@ -933,7 +982,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" s="14">
         <v>45103</v>
       </c>
@@ -941,10 +990,10 @@
         <v>2620</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="17">
         <v>45103</v>
       </c>
@@ -953,10 +1002,10 @@
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="14">
         <v>45103</v>
       </c>
@@ -967,7 +1016,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="17">
         <v>45103</v>
       </c>
@@ -979,7 +1028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A6" s="14">
         <v>45103</v>
       </c>
@@ -987,10 +1036,10 @@
         <v>1430</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A7" s="17">
         <v>45103</v>
       </c>
@@ -999,10 +1048,10 @@
         <v>1430</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A8" s="14">
         <v>45103</v>
       </c>
@@ -1013,7 +1062,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A9" s="17">
         <v>45103</v>
       </c>
@@ -1022,10 +1071,10 @@
         <v>1430</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A10" s="14">
         <v>45103</v>
       </c>
@@ -1033,10 +1082,10 @@
         <v>150</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A11" s="17">
         <v>45117</v>
       </c>
@@ -1045,52 +1094,101 @@
         <v>150</v>
       </c>
       <c r="D11" s="20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A12" s="14">
+        <v>45138</v>
+      </c>
+      <c r="C12" s="16">
+        <v>150</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="16"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
       <c r="D13" s="20"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
       <c r="C14" s="16"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="16"/>
-    </row>
-    <row r="17" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+    <row r="16" spans="1:4" ht="16.8" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22">
-        <f>SUM(B2:C17)</f>
-        <v>2940</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D19" s="24" t="s">
+      <c r="B16" s="22"/>
+      <c r="C16" s="22">
+        <f>SUM(B2:C15)</f>
+        <v>3090</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D17" s="24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="14">
+        <v>45145</v>
+      </c>
+      <c r="C21" s="26">
+        <v>150</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A22" s="17">
+        <v>45173</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="27">
+        <v>300</v>
+      </c>
+      <c r="D22" s="20" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="16.8" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22">
+        <f>SUM(C21:C22)</f>
+        <v>450</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
start 2023 Q4 and update details
</commit_message>
<xml_diff>
--- a/2023_Q3/2023-Q3_羽球季打費用明細.xlsx
+++ b/2023_Q3/2023-Q3_羽球季打費用明細.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alias\Documents\Docs\Private\週一豐東羽球團\2023_Q3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD76525A-4A98-4391-A1CF-41045DB91E03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF4137B-8080-48D1-B90B-74304E20BA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-88" yWindow="0" windowWidth="11484" windowHeight="12085" tabRatio="738" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
+    <workbookView xWindow="-106" yWindow="-106" windowWidth="22828" windowHeight="12209" tabRatio="738" activeTab="1" xr2:uid="{8981F119-1F50-4E2E-B5FC-EDE94F1AD592}"/>
   </bookViews>
   <sheets>
     <sheet name="2023Q3羽球季費資訊" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>豐東場地費1900-2100時段 $420/小時</t>
   </si>
@@ -177,46 +177,43 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>現金 Ivy友(Wendy) 臨打費</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>現金 Frank友(鎮豪) 臨打費</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>現金 Frank友(鎮豪) 臨打費</t>
-  </si>
-  <si>
-    <t>現金 香菇、香菇友臨打費 (請鉉竣代收)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>應收</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>現金 偉群 臨打費 (未收)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>=SUM(C21:C22)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2023/09/10 更新餘額</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>=SUM(B2:C15)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>7.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>!! 08/07 當日整團請假，09/04 得知球場規定未能補打本季也即將結束，由 Ivy 額外提供兩桶新球為補償</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 Ivy友(Wendy) 06/26臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 Frank友(鎮豪) 07/10臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 Frank友(鎮豪) 07/31臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 香菇、香菇友 09/04臨打費 (09/04請鉉竣代收)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 Frank友(鎮豪) 09/11臨打費</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>現金 偉群 08/07臨打費 (09/09請夜市代收)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>=SUM(B2:C16)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023/09/14 更新餘額</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -230,7 +227,7 @@
     <numFmt numFmtId="177" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -324,13 +321,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
-      <name val="Microsoft JhengHei UI"/>
-      <family val="2"/>
-      <charset val="136"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="5" tint="-0.249977111117893"/>
       <name val="Microsoft JhengHei UI"/>
       <family val="2"/>
       <charset val="136"/>
@@ -382,7 +372,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -460,12 +450,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -867,7 +851,7 @@
     </row>
     <row r="15" spans="1:3" ht="32.700000000000003" x14ac:dyDescent="0.4">
       <c r="A15" s="25" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -935,7 +919,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="5"/>
@@ -954,10 +938,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCCEF2F-70B8-4CD5-8F32-AA2B6924B187}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.350000000000001" x14ac:dyDescent="0.4"/>
@@ -1082,7 +1066,7 @@
         <v>150</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -1094,7 +1078,7 @@
         <v>150</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
@@ -1105,90 +1089,63 @@
         <v>150</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" s="17"/>
+      <c r="A13" s="17">
+        <v>45180</v>
+      </c>
       <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="19">
+        <v>300</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="C14" s="16"/>
-    </row>
-    <row r="15" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="17"/>
+      <c r="A14" s="14">
+        <v>45180</v>
+      </c>
+      <c r="C14" s="16">
+        <v>150</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A15" s="17">
+        <v>45183</v>
+      </c>
       <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="20"/>
-    </row>
-    <row r="16" spans="1:4" ht="16.8" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="21" t="s">
+      <c r="C15" s="19">
+        <v>150</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="C16" s="16"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.8" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22">
-        <f>SUM(B2:C15)</f>
-        <v>3090</v>
-      </c>
-      <c r="D16" s="23" t="s">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22">
+        <f>SUM(B2:C16)</f>
+        <v>3690</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="D17" s="24" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="14">
-        <v>45145</v>
-      </c>
-      <c r="C21" s="26">
-        <v>150</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="16.8" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="17">
-        <v>45173</v>
-      </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="27">
-        <v>300</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="16.8" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22">
-        <f>SUM(C21:C22)</f>
-        <v>450</v>
-      </c>
-      <c r="D23" s="23" t="s">
-        <v>44</v>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D18" s="24" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>